<commit_message>
student conflict with debugger
</commit_message>
<xml_diff>
--- a/Possible_Schedule.xlsx
+++ b/Possible_Schedule.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27307"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Downloads\COOP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3424AA6C-7038-4168-9328-AE03BEB92A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7E5DE72-42E0-4A9D-9C9E-F703E82BCE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2691,7 +2686,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3054,11 +3049,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
@@ -3066,7 +3061,7 @@
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3098,7 +3093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3130,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3162,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3194,7 +3189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3226,7 +3221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3258,7 +3253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3290,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -3322,7 +3317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -3354,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3386,7 +3381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3418,7 +3413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3450,7 +3445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3482,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3514,7 +3509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3546,7 +3541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -3578,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -3610,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -3642,7 +3637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -3674,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -3706,7 +3701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -3726,19 +3721,19 @@
         <v>80</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -3758,19 +3753,19 @@
         <v>83</v>
       </c>
       <c r="G22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
         <v>84</v>
       </c>
       <c r="I22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -3802,7 +3797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -3834,7 +3829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -3866,7 +3861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -3898,7 +3893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -3930,7 +3925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -3962,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>101</v>
       </c>
@@ -3994,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -4026,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -4058,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -4090,7 +4085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -4122,7 +4117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -4154,7 +4149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>119</v>
       </c>
@@ -4186,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>123</v>
       </c>
@@ -4218,7 +4213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -4250,7 +4245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -4282,7 +4277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>131</v>
       </c>
@@ -4314,7 +4309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -4346,7 +4341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -4378,7 +4373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>139</v>
       </c>
@@ -4410,7 +4405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -4442,7 +4437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>145</v>
       </c>
@@ -4474,7 +4469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>149</v>
       </c>
@@ -4506,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>152</v>
       </c>
@@ -4538,7 +4533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>154</v>
       </c>
@@ -4558,19 +4553,19 @@
         <v>83</v>
       </c>
       <c r="G47">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H47" t="s">
         <v>88</v>
       </c>
       <c r="I47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J47">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>156</v>
       </c>
@@ -4602,7 +4597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -4634,7 +4629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>160</v>
       </c>
@@ -4666,7 +4661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>162</v>
       </c>
@@ -4698,7 +4693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>165</v>
       </c>
@@ -4730,7 +4725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>169</v>
       </c>
@@ -4762,7 +4757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>171</v>
       </c>
@@ -4794,7 +4789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>174</v>
       </c>
@@ -4826,7 +4821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>176</v>
       </c>
@@ -4858,7 +4853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>178</v>
       </c>
@@ -4890,7 +4885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>182</v>
       </c>
@@ -4922,7 +4917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>186</v>
       </c>
@@ -4954,7 +4949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>189</v>
       </c>
@@ -4986,7 +4981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>193</v>
       </c>
@@ -5018,7 +5013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>197</v>
       </c>
@@ -5050,7 +5045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>199</v>
       </c>
@@ -5082,7 +5077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>202</v>
       </c>
@@ -5114,7 +5109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>205</v>
       </c>
@@ -5146,7 +5141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>208</v>
       </c>
@@ -5178,7 +5173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>211</v>
       </c>
@@ -5210,7 +5205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>213</v>
       </c>
@@ -5242,7 +5237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>215</v>
       </c>
@@ -5274,7 +5269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>217</v>
       </c>
@@ -5306,7 +5301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>220</v>
       </c>
@@ -5338,7 +5333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -5370,7 +5365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>225</v>
       </c>
@@ -5402,7 +5397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>228</v>
       </c>
@@ -5434,7 +5429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>231</v>
       </c>
@@ -5466,7 +5461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -5498,7 +5493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>235</v>
       </c>
@@ -5530,7 +5525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>236</v>
       </c>
@@ -5562,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>238</v>
       </c>
@@ -5594,7 +5589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>241</v>
       </c>
@@ -5626,7 +5621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>244</v>
       </c>
@@ -5658,7 +5653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>247</v>
       </c>
@@ -5690,7 +5685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>250</v>
       </c>
@@ -5722,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>252</v>
       </c>
@@ -5754,7 +5749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>254</v>
       </c>
@@ -5786,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>256</v>
       </c>
@@ -5818,7 +5813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>260</v>
       </c>
@@ -5850,7 +5845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>262</v>
       </c>
@@ -5882,7 +5877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>265</v>
       </c>
@@ -5914,7 +5909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>269</v>
       </c>
@@ -5946,7 +5941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>272</v>
       </c>
@@ -5978,7 +5973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>275</v>
       </c>
@@ -6010,7 +6005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>279</v>
       </c>
@@ -6042,7 +6037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>281</v>
       </c>
@@ -6074,7 +6069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>283</v>
       </c>
@@ -6106,7 +6101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>286</v>
       </c>
@@ -6138,7 +6133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>289</v>
       </c>
@@ -6170,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>292</v>
       </c>
@@ -6202,7 +6197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>295</v>
       </c>
@@ -6234,7 +6229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -6266,7 +6261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>301</v>
       </c>
@@ -6298,7 +6293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>304</v>
       </c>
@@ -6330,7 +6325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>306</v>
       </c>
@@ -6362,7 +6357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
         <v>309</v>
       </c>
@@ -6394,7 +6389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
         <v>314</v>
       </c>
@@ -6426,7 +6421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>318</v>
       </c>
@@ -6458,7 +6453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>320</v>
       </c>
@@ -6490,7 +6485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
         <v>323</v>
       </c>
@@ -6522,7 +6517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
         <v>324</v>
       </c>
@@ -6554,7 +6549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
         <v>327</v>
       </c>
@@ -6586,7 +6581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>329</v>
       </c>
@@ -6618,7 +6613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>331</v>
       </c>
@@ -6650,7 +6645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>334</v>
       </c>
@@ -6682,7 +6677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>336</v>
       </c>
@@ -6714,7 +6709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>338</v>
       </c>
@@ -6746,7 +6741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>341</v>
       </c>
@@ -6778,7 +6773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>345</v>
       </c>
@@ -6810,7 +6805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>349</v>
       </c>
@@ -6842,7 +6837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>352</v>
       </c>
@@ -6874,7 +6869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
         <v>354</v>
       </c>
@@ -6906,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" t="s">
         <v>357</v>
       </c>
@@ -6938,7 +6933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
         <v>359</v>
       </c>
@@ -6970,7 +6965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
         <v>362</v>
       </c>
@@ -7002,7 +6997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" t="s">
         <v>364</v>
       </c>
@@ -7034,7 +7029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" t="s">
         <v>365</v>
       </c>
@@ -7066,7 +7061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" t="s">
         <v>367</v>
       </c>
@@ -7098,7 +7093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" t="s">
         <v>369</v>
       </c>
@@ -7130,7 +7125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" t="s">
         <v>371</v>
       </c>
@@ -7162,7 +7157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" t="s">
         <v>373</v>
       </c>
@@ -7194,7 +7189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" t="s">
         <v>375</v>
       </c>
@@ -7226,7 +7221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" t="s">
         <v>377</v>
       </c>
@@ -7258,7 +7253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" t="s">
         <v>381</v>
       </c>
@@ -7290,7 +7285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" t="s">
         <v>382</v>
       </c>
@@ -7322,7 +7317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" t="s">
         <v>385</v>
       </c>
@@ -7354,7 +7349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" t="s">
         <v>388</v>
       </c>
@@ -7386,7 +7381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" t="s">
         <v>391</v>
       </c>
@@ -7418,7 +7413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" t="s">
         <v>392</v>
       </c>
@@ -7450,7 +7445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" t="s">
         <v>395</v>
       </c>
@@ -7482,7 +7477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" t="s">
         <v>399</v>
       </c>
@@ -7514,7 +7509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" t="s">
         <v>401</v>
       </c>
@@ -7546,7 +7541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" t="s">
         <v>405</v>
       </c>
@@ -7578,7 +7573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" t="s">
         <v>408</v>
       </c>
@@ -7610,7 +7605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" t="s">
         <v>410</v>
       </c>
@@ -7642,7 +7637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" t="s">
         <v>412</v>
       </c>
@@ -7674,7 +7669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" t="s">
         <v>414</v>
       </c>
@@ -7706,7 +7701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" t="s">
         <v>416</v>
       </c>
@@ -7738,7 +7733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" t="s">
         <v>417</v>
       </c>
@@ -7770,7 +7765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" t="s">
         <v>418</v>
       </c>
@@ -7802,7 +7797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" t="s">
         <v>420</v>
       </c>
@@ -7834,7 +7829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" t="s">
         <v>422</v>
       </c>
@@ -7866,7 +7861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" t="s">
         <v>423</v>
       </c>
@@ -7898,7 +7893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" t="s">
         <v>425</v>
       </c>
@@ -7930,7 +7925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" t="s">
         <v>426</v>
       </c>
@@ -7962,7 +7957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" t="s">
         <v>428</v>
       </c>
@@ -7994,7 +7989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" t="s">
         <v>430</v>
       </c>
@@ -8026,7 +8021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" t="s">
         <v>433</v>
       </c>
@@ -8058,7 +8053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" t="s">
         <v>434</v>
       </c>
@@ -8090,7 +8085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" t="s">
         <v>435</v>
       </c>
@@ -8122,7 +8117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" t="s">
         <v>437</v>
       </c>
@@ -8154,7 +8149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" t="s">
         <v>439</v>
       </c>
@@ -8186,7 +8181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" t="s">
         <v>442</v>
       </c>
@@ -8218,7 +8213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" t="s">
         <v>443</v>
       </c>
@@ -8250,7 +8245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" t="s">
         <v>446</v>
       </c>
@@ -8282,7 +8277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" t="s">
         <v>449</v>
       </c>
@@ -8314,7 +8309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" t="s">
         <v>451</v>
       </c>
@@ -8346,7 +8341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" t="s">
         <v>454</v>
       </c>
@@ -8378,7 +8373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" t="s">
         <v>457</v>
       </c>
@@ -8410,7 +8405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" t="s">
         <v>459</v>
       </c>
@@ -8442,7 +8437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" t="s">
         <v>461</v>
       </c>
@@ -8474,7 +8469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" t="s">
         <v>463</v>
       </c>
@@ -8506,7 +8501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" t="s">
         <v>465</v>
       </c>
@@ -8538,7 +8533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" t="s">
         <v>466</v>
       </c>
@@ -8570,7 +8565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" t="s">
         <v>468</v>
       </c>
@@ -8602,7 +8597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" t="s">
         <v>470</v>
       </c>
@@ -8634,7 +8629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" t="s">
         <v>471</v>
       </c>
@@ -8666,7 +8661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" t="s">
         <v>472</v>
       </c>
@@ -8698,7 +8693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" t="s">
         <v>474</v>
       </c>
@@ -8730,7 +8725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" t="s">
         <v>476</v>
       </c>
@@ -8762,7 +8757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" t="s">
         <v>478</v>
       </c>
@@ -8794,7 +8789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" t="s">
         <v>480</v>
       </c>
@@ -8826,7 +8821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" t="s">
         <v>481</v>
       </c>
@@ -8858,7 +8853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" t="s">
         <v>484</v>
       </c>
@@ -8890,7 +8885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" t="s">
         <v>486</v>
       </c>
@@ -8922,7 +8917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" t="s">
         <v>488</v>
       </c>
@@ -8954,7 +8949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" t="s">
         <v>490</v>
       </c>
@@ -8986,7 +8981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" t="s">
         <v>491</v>
       </c>
@@ -9018,7 +9013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" t="s">
         <v>492</v>
       </c>
@@ -9050,7 +9045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" t="s">
         <v>493</v>
       </c>
@@ -9082,7 +9077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" t="s">
         <v>495</v>
       </c>
@@ -9114,7 +9109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" t="s">
         <v>496</v>
       </c>
@@ -9146,7 +9141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" t="s">
         <v>499</v>
       </c>
@@ -9178,7 +9173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" t="s">
         <v>501</v>
       </c>
@@ -9210,7 +9205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" t="s">
         <v>503</v>
       </c>
@@ -9242,7 +9237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" t="s">
         <v>506</v>
       </c>
@@ -9274,7 +9269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" t="s">
         <v>509</v>
       </c>
@@ -9306,7 +9301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" t="s">
         <v>510</v>
       </c>
@@ -9338,7 +9333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" t="s">
         <v>511</v>
       </c>
@@ -9370,7 +9365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" t="s">
         <v>512</v>
       </c>
@@ -9402,7 +9397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" t="s">
         <v>514</v>
       </c>
@@ -9434,7 +9429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" t="s">
         <v>516</v>
       </c>
@@ -9466,7 +9461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" t="s">
         <v>518</v>
       </c>
@@ -9498,7 +9493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" t="s">
         <v>520</v>
       </c>
@@ -9530,7 +9525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" t="s">
         <v>522</v>
       </c>
@@ -9562,7 +9557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" t="s">
         <v>524</v>
       </c>
@@ -9594,7 +9589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" t="s">
         <v>526</v>
       </c>
@@ -9626,7 +9621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" t="s">
         <v>528</v>
       </c>
@@ -9658,7 +9653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" t="s">
         <v>531</v>
       </c>
@@ -9690,7 +9685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" t="s">
         <v>534</v>
       </c>
@@ -9722,7 +9717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" t="s">
         <v>536</v>
       </c>
@@ -9754,7 +9749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" t="s">
         <v>539</v>
       </c>
@@ -9786,7 +9781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" t="s">
         <v>540</v>
       </c>
@@ -9818,7 +9813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" t="s">
         <v>543</v>
       </c>
@@ -9850,7 +9845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" t="s">
         <v>545</v>
       </c>
@@ -9882,7 +9877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" t="s">
         <v>547</v>
       </c>
@@ -9914,7 +9909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" t="s">
         <v>549</v>
       </c>
@@ -9946,7 +9941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" t="s">
         <v>552</v>
       </c>
@@ -9978,7 +9973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" t="s">
         <v>554</v>
       </c>
@@ -10010,7 +10005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" t="s">
         <v>557</v>
       </c>
@@ -10042,7 +10037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" t="s">
         <v>558</v>
       </c>
@@ -10074,7 +10069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" t="s">
         <v>561</v>
       </c>
@@ -10106,7 +10101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" t="s">
         <v>563</v>
       </c>
@@ -10138,7 +10133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" t="s">
         <v>565</v>
       </c>
@@ -10170,7 +10165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" t="s">
         <v>567</v>
       </c>
@@ -10202,7 +10197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" t="s">
         <v>569</v>
       </c>
@@ -10234,7 +10229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" t="s">
         <v>570</v>
       </c>
@@ -10266,7 +10261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" t="s">
         <v>574</v>
       </c>
@@ -10298,7 +10293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" t="s">
         <v>576</v>
       </c>
@@ -10330,7 +10325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" t="s">
         <v>579</v>
       </c>
@@ -10362,7 +10357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" t="s">
         <v>581</v>
       </c>
@@ -10394,7 +10389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" t="s">
         <v>584</v>
       </c>
@@ -10426,7 +10421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" t="s">
         <v>585</v>
       </c>
@@ -10458,7 +10453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" t="s">
         <v>586</v>
       </c>
@@ -10490,7 +10485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" t="s">
         <v>588</v>
       </c>
@@ -10522,7 +10517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" t="s">
         <v>592</v>
       </c>
@@ -10554,7 +10549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" t="s">
         <v>594</v>
       </c>
@@ -10586,7 +10581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" t="s">
         <v>596</v>
       </c>
@@ -10618,7 +10613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" t="s">
         <v>598</v>
       </c>
@@ -10650,7 +10645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" t="s">
         <v>599</v>
       </c>
@@ -10682,7 +10677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" t="s">
         <v>600</v>
       </c>
@@ -10714,7 +10709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" t="s">
         <v>603</v>
       </c>
@@ -10746,7 +10741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" t="s">
         <v>606</v>
       </c>
@@ -10778,7 +10773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" t="s">
         <v>607</v>
       </c>
@@ -10810,7 +10805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" t="s">
         <v>609</v>
       </c>
@@ -10842,7 +10837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" t="s">
         <v>610</v>
       </c>
@@ -10874,7 +10869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" t="s">
         <v>612</v>
       </c>
@@ -10906,7 +10901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" t="s">
         <v>615</v>
       </c>
@@ -10938,7 +10933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" t="s">
         <v>617</v>
       </c>
@@ -10970,7 +10965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" t="s">
         <v>620</v>
       </c>
@@ -11002,7 +10997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" t="s">
         <v>622</v>
       </c>
@@ -11034,7 +11029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" t="s">
         <v>627</v>
       </c>
@@ -11066,7 +11061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" t="s">
         <v>630</v>
       </c>
@@ -11098,7 +11093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" t="s">
         <v>633</v>
       </c>
@@ -11130,7 +11125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" t="s">
         <v>635</v>
       </c>
@@ -11162,7 +11157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" t="s">
         <v>637</v>
       </c>
@@ -11194,7 +11189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" t="s">
         <v>639</v>
       </c>
@@ -11226,7 +11221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" t="s">
         <v>641</v>
       </c>
@@ -11258,7 +11253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" t="s">
         <v>643</v>
       </c>
@@ -11290,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" t="s">
         <v>645</v>
       </c>
@@ -11322,7 +11317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" t="s">
         <v>647</v>
       </c>
@@ -11354,7 +11349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" t="s">
         <v>649</v>
       </c>
@@ -11386,7 +11381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" t="s">
         <v>652</v>
       </c>
@@ -11418,7 +11413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" t="s">
         <v>655</v>
       </c>
@@ -11450,7 +11445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" t="s">
         <v>658</v>
       </c>
@@ -11482,7 +11477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" t="s">
         <v>660</v>
       </c>
@@ -11514,7 +11509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" t="s">
         <v>662</v>
       </c>
@@ -11546,7 +11541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" t="s">
         <v>664</v>
       </c>
@@ -11578,7 +11573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" t="s">
         <v>666</v>
       </c>
@@ -11610,7 +11605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" t="s">
         <v>667</v>
       </c>
@@ -11642,7 +11637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" t="s">
         <v>668</v>
       </c>
@@ -11674,7 +11669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" t="s">
         <v>669</v>
       </c>
@@ -11706,7 +11701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" t="s">
         <v>671</v>
       </c>
@@ -11738,7 +11733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" t="s">
         <v>672</v>
       </c>
@@ -11770,7 +11765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" t="s">
         <v>675</v>
       </c>
@@ -11802,7 +11797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" t="s">
         <v>677</v>
       </c>
@@ -11834,7 +11829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" t="s">
         <v>679</v>
       </c>
@@ -11866,7 +11861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" t="s">
         <v>682</v>
       </c>
@@ -11898,7 +11893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" t="s">
         <v>684</v>
       </c>
@@ -11930,7 +11925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" t="s">
         <v>686</v>
       </c>
@@ -11962,7 +11957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" t="s">
         <v>688</v>
       </c>
@@ -11994,7 +11989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" t="s">
         <v>689</v>
       </c>
@@ -12026,7 +12021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" t="s">
         <v>692</v>
       </c>
@@ -12058,7 +12053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" t="s">
         <v>695</v>
       </c>
@@ -12090,7 +12085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" t="s">
         <v>697</v>
       </c>
@@ -12122,7 +12117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" t="s">
         <v>701</v>
       </c>
@@ -12154,7 +12149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" t="s">
         <v>704</v>
       </c>
@@ -12186,7 +12181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" t="s">
         <v>707</v>
       </c>
@@ -12218,7 +12213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" t="s">
         <v>709</v>
       </c>
@@ -12250,7 +12245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" t="s">
         <v>710</v>
       </c>
@@ -12282,7 +12277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" t="s">
         <v>712</v>
       </c>
@@ -12314,7 +12309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" t="s">
         <v>714</v>
       </c>
@@ -12346,7 +12341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" t="s">
         <v>718</v>
       </c>
@@ -12378,7 +12373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" t="s">
         <v>721</v>
       </c>
@@ -12410,7 +12405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10">
       <c r="A293" t="s">
         <v>723</v>
       </c>
@@ -12442,7 +12437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10">
       <c r="A294" t="s">
         <v>726</v>
       </c>
@@ -12474,7 +12469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10">
       <c r="A295" t="s">
         <v>728</v>
       </c>
@@ -12506,7 +12501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10">
       <c r="A296" t="s">
         <v>731</v>
       </c>
@@ -12538,7 +12533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10">
       <c r="A297" t="s">
         <v>733</v>
       </c>
@@ -12570,7 +12565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10">
       <c r="A298" t="s">
         <v>736</v>
       </c>
@@ -12602,7 +12597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10">
       <c r="A299" t="s">
         <v>738</v>
       </c>
@@ -12634,7 +12629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10">
       <c r="A300" t="s">
         <v>740</v>
       </c>
@@ -12666,7 +12661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10">
       <c r="A301" t="s">
         <v>743</v>
       </c>
@@ -12698,7 +12693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10">
       <c r="A302" t="s">
         <v>746</v>
       </c>
@@ -12730,7 +12725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10">
       <c r="A303" t="s">
         <v>748</v>
       </c>
@@ -12762,7 +12757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10">
       <c r="A304" t="s">
         <v>750</v>
       </c>
@@ -12794,7 +12789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10">
       <c r="A305" t="s">
         <v>753</v>
       </c>
@@ -12826,7 +12821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10">
       <c r="A306" t="s">
         <v>754</v>
       </c>
@@ -12858,7 +12853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10">
       <c r="A307" t="s">
         <v>756</v>
       </c>
@@ -12890,7 +12885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10">
       <c r="A308" t="s">
         <v>758</v>
       </c>
@@ -12922,7 +12917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10">
       <c r="A309" t="s">
         <v>760</v>
       </c>
@@ -12954,7 +12949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10">
       <c r="A310" t="s">
         <v>762</v>
       </c>
@@ -12986,7 +12981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10">
       <c r="A311" t="s">
         <v>764</v>
       </c>
@@ -13018,7 +13013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10">
       <c r="A312" t="s">
         <v>765</v>
       </c>
@@ -13050,7 +13045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10">
       <c r="A313" t="s">
         <v>767</v>
       </c>
@@ -13082,7 +13077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10">
       <c r="A314" t="s">
         <v>768</v>
       </c>
@@ -13114,7 +13109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10">
       <c r="A315" t="s">
         <v>769</v>
       </c>
@@ -13146,7 +13141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10">
       <c r="A316" t="s">
         <v>770</v>
       </c>
@@ -13178,7 +13173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10">
       <c r="A317" t="s">
         <v>772</v>
       </c>
@@ -13210,7 +13205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10">
       <c r="A318" t="s">
         <v>774</v>
       </c>
@@ -13242,7 +13237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10">
       <c r="A319" t="s">
         <v>776</v>
       </c>
@@ -13274,7 +13269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10">
       <c r="A320" t="s">
         <v>778</v>
       </c>
@@ -13306,7 +13301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10">
       <c r="A321" t="s">
         <v>780</v>
       </c>
@@ -13338,7 +13333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10">
       <c r="A322" t="s">
         <v>782</v>
       </c>
@@ -13370,7 +13365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10">
       <c r="A323" t="s">
         <v>784</v>
       </c>
@@ -13402,7 +13397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10">
       <c r="A324" t="s">
         <v>785</v>
       </c>
@@ -13434,7 +13429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10">
       <c r="A325" t="s">
         <v>789</v>
       </c>
@@ -13466,7 +13461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10">
       <c r="A326" t="s">
         <v>792</v>
       </c>
@@ -13498,7 +13493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10">
       <c r="A327" t="s">
         <v>793</v>
       </c>
@@ -13530,7 +13525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10">
       <c r="A328" t="s">
         <v>795</v>
       </c>
@@ -13562,7 +13557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10">
       <c r="A329" t="s">
         <v>797</v>
       </c>
@@ -13594,7 +13589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10">
       <c r="A330" t="s">
         <v>800</v>
       </c>
@@ -13626,7 +13621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10">
       <c r="A331" t="s">
         <v>802</v>
       </c>
@@ -13658,7 +13653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10">
       <c r="A332" t="s">
         <v>804</v>
       </c>
@@ -13690,7 +13685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10">
       <c r="A333" t="s">
         <v>806</v>
       </c>
@@ -13722,7 +13717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10">
       <c r="A334" t="s">
         <v>809</v>
       </c>
@@ -13754,7 +13749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10">
       <c r="A335" t="s">
         <v>812</v>
       </c>
@@ -13786,7 +13781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10">
       <c r="A336" t="s">
         <v>814</v>
       </c>
@@ -13818,7 +13813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10">
       <c r="A337" t="s">
         <v>817</v>
       </c>
@@ -13850,7 +13845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10">
       <c r="A338" t="s">
         <v>820</v>
       </c>
@@ -13882,7 +13877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10">
       <c r="A339" t="s">
         <v>821</v>
       </c>
@@ -13914,7 +13909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10">
       <c r="A340" t="s">
         <v>823</v>
       </c>
@@ -13946,7 +13941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10">
       <c r="A341" t="s">
         <v>825</v>
       </c>
@@ -13978,7 +13973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10">
       <c r="A342" t="s">
         <v>827</v>
       </c>
@@ -14010,7 +14005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10">
       <c r="A343" t="s">
         <v>830</v>
       </c>
@@ -14042,7 +14037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10">
       <c r="A344" t="s">
         <v>833</v>
       </c>
@@ -14074,7 +14069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10">
       <c r="A345" t="s">
         <v>835</v>
       </c>
@@ -14106,7 +14101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10">
       <c r="A346" t="s">
         <v>838</v>
       </c>
@@ -14138,7 +14133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10">
       <c r="A347" t="s">
         <v>839</v>
       </c>
@@ -14170,7 +14165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10">
       <c r="A348" t="s">
         <v>841</v>
       </c>
@@ -14202,7 +14197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10">
       <c r="A349" t="s">
         <v>842</v>
       </c>
@@ -14234,7 +14229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10">
       <c r="A350" t="s">
         <v>844</v>
       </c>
@@ -14266,7 +14261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10">
       <c r="A351" t="s">
         <v>845</v>
       </c>
@@ -14298,7 +14293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10">
       <c r="A352" t="s">
         <v>847</v>
       </c>
@@ -14330,7 +14325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10">
       <c r="A353" t="s">
         <v>848</v>
       </c>
@@ -14362,7 +14357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10">
       <c r="A354" t="s">
         <v>849</v>
       </c>
@@ -14394,7 +14389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10">
       <c r="A355" t="s">
         <v>850</v>
       </c>
@@ -14426,7 +14421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10">
       <c r="A356" t="s">
         <v>853</v>
       </c>
@@ -14458,7 +14453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10">
       <c r="A357" t="s">
         <v>855</v>
       </c>
@@ -14490,7 +14485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10">
       <c r="A358" t="s">
         <v>857</v>
       </c>
@@ -14522,7 +14517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10">
       <c r="A359" t="s">
         <v>859</v>
       </c>
@@ -14554,7 +14549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10">
       <c r="A360" t="s">
         <v>862</v>
       </c>
@@ -14586,7 +14581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10">
       <c r="A361" t="s">
         <v>864</v>
       </c>
@@ -14618,7 +14613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10">
       <c r="A362" t="s">
         <v>866</v>
       </c>
@@ -14650,7 +14645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10">
       <c r="A363" t="s">
         <v>868</v>
       </c>
@@ -14682,7 +14677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10">
       <c r="A364" t="s">
         <v>871</v>
       </c>
@@ -14714,7 +14709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10">
       <c r="A365" t="s">
         <v>873</v>
       </c>
@@ -14746,7 +14741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10">
       <c r="A366" t="s">
         <v>875</v>
       </c>
@@ -14778,7 +14773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10">
       <c r="A367" t="s">
         <v>878</v>
       </c>
@@ -14810,7 +14805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10">
       <c r="A368" t="s">
         <v>880</v>
       </c>
@@ -14842,7 +14837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10">
       <c r="A369" t="s">
         <v>881</v>
       </c>

</xml_diff>